<commit_message>
Salva nova Tabela e relatorio
</commit_message>
<xml_diff>
--- a/tabela.xlsx
+++ b/tabela.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vitor\Desktop\livros da faculdade\AEDS 2\TrabalhoArvAVL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3122E512-7B4B-4F91-9CBD-665A2F58D58F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{318F2336-6D82-4B82-A983-73102BEDE941}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{F07C88E9-8C01-47CF-85DE-71F8B0B86510}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>10k</t>
   </si>
@@ -85,6 +85,63 @@
   </si>
   <si>
     <t>100k</t>
+  </si>
+  <si>
+    <t>10-20k</t>
+  </si>
+  <si>
+    <t>20-30k</t>
+  </si>
+  <si>
+    <t>30-40k</t>
+  </si>
+  <si>
+    <t>40-50k</t>
+  </si>
+  <si>
+    <t>50-60k</t>
+  </si>
+  <si>
+    <t>60-70k</t>
+  </si>
+  <si>
+    <t>70-80k</t>
+  </si>
+  <si>
+    <t>80-90k</t>
+  </si>
+  <si>
+    <t>90-100k</t>
+  </si>
+  <si>
+    <t>100-110k</t>
+  </si>
+  <si>
+    <t>110-120k</t>
+  </si>
+  <si>
+    <t>120-130k</t>
+  </si>
+  <si>
+    <t>130-140k</t>
+  </si>
+  <si>
+    <t>140-150k</t>
+  </si>
+  <si>
+    <t>150-160k</t>
+  </si>
+  <si>
+    <t>160-170k</t>
+  </si>
+  <si>
+    <t>170-180k</t>
+  </si>
+  <si>
+    <t>180-190k</t>
+  </si>
+  <si>
+    <t>190-200k</t>
   </si>
 </sst>
 </file>
@@ -279,64 +336,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>13957</c:v>
+                  <c:v>13986</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27725</c:v>
+                  <c:v>28016</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41319</c:v>
+                  <c:v>41936</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>54890</c:v>
+                  <c:v>55920</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>67995</c:v>
+                  <c:v>69808</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>81333</c:v>
+                  <c:v>83859</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>94330</c:v>
+                  <c:v>97580</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>107177</c:v>
+                  <c:v>111318</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>119966</c:v>
+                  <c:v>125078</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>132246</c:v>
+                  <c:v>139142</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>144684</c:v>
+                  <c:v>152725</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>156919</c:v>
+                  <c:v>166586</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>168925</c:v>
+                  <c:v>180102</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>181070</c:v>
+                  <c:v>193922</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>192808</c:v>
+                  <c:v>207486</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>204647</c:v>
+                  <c:v>220980</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>215736</c:v>
+                  <c:v>234619</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>227416</c:v>
+                  <c:v>247859</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>238543</c:v>
+                  <c:v>261573</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>250026</c:v>
+                  <c:v>274927</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -558,86 +615,96 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
-      <c:areaChart>
-        <c:grouping val="stacked"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.4862348172715352E-2"/>
+          <c:y val="0.14945399857240274"/>
+          <c:w val="0.91021905272542447"/>
+          <c:h val="0.71146962273799508"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:cat>
             <c:strRef>
               <c:f>Planilha1!$D$1:$D$20</c:f>
               <c:strCache>
-                <c:ptCount val="20"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>10k</c:v>
+                  <c:v>10-20k</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20k</c:v>
+                  <c:v>20-30k</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30k</c:v>
+                  <c:v>30-40k</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40k</c:v>
+                  <c:v>40-50k</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50k</c:v>
+                  <c:v>50-60k</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>60k</c:v>
+                  <c:v>60-70k</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>70k</c:v>
+                  <c:v>70-80k</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>80k</c:v>
+                  <c:v>80-90k</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>90k</c:v>
+                  <c:v>90-100k</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>100k</c:v>
+                  <c:v>100-110k</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>110k</c:v>
+                  <c:v>110-120k</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>120k</c:v>
+                  <c:v>120-130k</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>130k</c:v>
+                  <c:v>130-140k</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>140k</c:v>
+                  <c:v>140-150k</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>150k</c:v>
+                  <c:v>150-160k</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>160k</c:v>
+                  <c:v>160-170k</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>170k</c:v>
+                  <c:v>170-180k</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>180k</c:v>
+                  <c:v>180-190k</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>190k</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>200k</c:v>
+                  <c:v>190-200k</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -649,65 +716,66 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>98.645840796732813</c:v>
+                  <c:v>100.31460031460031</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>49.031559963931471</c:v>
+                  <c:v>49.685893774985722</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>32.844454125220842</c:v>
+                  <c:v>33.34605112552461</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23.875022772818362</c:v>
+                  <c:v>24.835479256080113</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>19.616148246194573</c:v>
+                  <c:v>20.128065551226221</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>15.979983524522643</c:v>
+                  <c:v>16.361988576062199</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13.619209159334252</c:v>
+                  <c:v>14.078704652592744</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11.932597478936714</c:v>
+                  <c:v>12.360983848074884</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10.236233599519865</c:v>
+                  <c:v>11.244183629415245</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.4051994011161018</c:v>
+                  <c:v>9.7619697862615169</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8.4563600674573554</c:v>
+                  <c:v>9.0757898183008674</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7.6510811310293843</c:v>
+                  <c:v>8.1135269470423683</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7.1895811750776968</c:v>
+                  <c:v>7.6734295010605109</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.4825757994145921</c:v>
+                  <c:v>6.9945648250327448</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6.1403053815194388</c:v>
+                  <c:v>6.5035713252942369</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5.4185988555903579</c:v>
+                  <c:v>6.1720517693908956</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5.414024548522268</c:v>
+                  <c:v>5.6431917278651778</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4.8927955816653181</c:v>
+                  <c:v>5.5329844790788316</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4.8138071542656879</c:v>
+                  <c:v>5.1052669809192848</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-7A5E-4513-8FDD-A5B30B07510D}"/>
@@ -722,9 +790,10 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:smooth val="0"/>
         <c:axId val="291920184"/>
         <c:axId val="291919200"/>
-      </c:areaChart>
+      </c:lineChart>
       <c:catAx>
         <c:axId val="291920184"/>
         <c:scaling>
@@ -830,11 +899,11 @@
         </c:txPr>
         <c:crossAx val="291920184"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="25400">
           <a:noFill/>
         </a:ln>
         <a:effectLst/>
@@ -2034,16 +2103,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>4761</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>157161</xdr:rowOff>
+      <xdr:rowOff>185736</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
+      <xdr:col>31</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2370,8 +2439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6B42CD4-EB4B-4A9B-824B-5DD0D724BEEA}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D19" sqref="D1:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2381,14 +2450,14 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>13957</v>
+        <v>13986</v>
       </c>
       <c r="D1" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E1">
         <f>( (B2 - B1) / B1 * 100)</f>
-        <v>98.645840796732813</v>
+        <v>100.31460031460031</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2396,14 +2465,14 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>27725</v>
+        <v>28016</v>
       </c>
       <c r="D2" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="E2">
         <f>((B3 - B2) / B2 * 100)</f>
-        <v>49.031559963931471</v>
+        <v>49.685893774985722</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2411,14 +2480,14 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>41319</v>
+        <v>41936</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="E3">
-        <f xml:space="preserve"> ((B4 - B3) / B3 * 100)</f>
-        <v>32.844454125220842</v>
+        <f t="shared" ref="E3:E19" si="0" xml:space="preserve"> ((B4 - B3) / B3 * 100)</f>
+        <v>33.34605112552461</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2426,14 +2495,14 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>54890</v>
+        <v>55920</v>
       </c>
       <c r="D4" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="E4">
-        <f xml:space="preserve"> ((B5 - B4) / B4 * 100)</f>
-        <v>23.875022772818362</v>
+        <f t="shared" si="0"/>
+        <v>24.835479256080113</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2441,14 +2510,14 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>67995</v>
+        <v>69808</v>
       </c>
       <c r="D5" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="E5">
-        <f xml:space="preserve"> ((B6 - B5) / B5 * 100)</f>
-        <v>19.616148246194573</v>
+        <f t="shared" si="0"/>
+        <v>20.128065551226221</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2456,14 +2525,14 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>81333</v>
+        <v>83859</v>
       </c>
       <c r="D6" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E6">
-        <f xml:space="preserve"> ((B7 - B6) / B6 * 100)</f>
-        <v>15.979983524522643</v>
+        <f t="shared" si="0"/>
+        <v>16.361988576062199</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2471,14 +2540,14 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>94330</v>
+        <v>97580</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="E7">
-        <f xml:space="preserve"> ((B8 - B7) / B7 * 100)</f>
-        <v>13.619209159334252</v>
+        <f t="shared" si="0"/>
+        <v>14.078704652592744</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -2486,14 +2555,14 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>107177</v>
+        <v>111318</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="E8">
-        <f xml:space="preserve"> ((B9 - B8) / B8 * 100)</f>
-        <v>11.932597478936714</v>
+        <f t="shared" si="0"/>
+        <v>12.360983848074884</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -2501,14 +2570,14 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>119966</v>
+        <v>125078</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="E9">
-        <f xml:space="preserve"> ((B10 - B9) / B9 * 100)</f>
-        <v>10.236233599519865</v>
+        <f t="shared" si="0"/>
+        <v>11.244183629415245</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2516,14 +2585,14 @@
         <v>19</v>
       </c>
       <c r="B10">
-        <v>132246</v>
+        <v>139142</v>
       </c>
       <c r="D10" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="E10">
-        <f xml:space="preserve"> ((B11 - B10) / B10 * 100)</f>
-        <v>9.4051994011161018</v>
+        <f t="shared" si="0"/>
+        <v>9.7619697862615169</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -2531,14 +2600,14 @@
         <v>18</v>
       </c>
       <c r="B11">
-        <v>144684</v>
+        <v>152725</v>
       </c>
       <c r="D11" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="E11">
-        <f xml:space="preserve"> ((B12 - B11) / B11 * 100)</f>
-        <v>8.4563600674573554</v>
+        <f t="shared" si="0"/>
+        <v>9.0757898183008674</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2546,14 +2615,14 @@
         <v>17</v>
       </c>
       <c r="B12">
-        <v>156919</v>
+        <v>166586</v>
       </c>
       <c r="D12" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="E12">
-        <f xml:space="preserve"> ((B13 - B12) / B12 * 100)</f>
-        <v>7.6510811310293843</v>
+        <f t="shared" si="0"/>
+        <v>8.1135269470423683</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2561,14 +2630,14 @@
         <v>16</v>
       </c>
       <c r="B13">
-        <v>168925</v>
+        <v>180102</v>
       </c>
       <c r="D13" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="E13">
-        <f xml:space="preserve"> ((B14 - B13) / B13 * 100)</f>
-        <v>7.1895811750776968</v>
+        <f t="shared" si="0"/>
+        <v>7.6734295010605109</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -2576,14 +2645,14 @@
         <v>15</v>
       </c>
       <c r="B14">
-        <v>181070</v>
+        <v>193922</v>
       </c>
       <c r="D14" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="E14">
-        <f xml:space="preserve"> ((B15 - B14) / B14 * 100)</f>
-        <v>6.4825757994145921</v>
+        <f t="shared" si="0"/>
+        <v>6.9945648250327448</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -2591,14 +2660,14 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>192808</v>
+        <v>207486</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="E15">
-        <f xml:space="preserve"> ((B16 - B15) / B15 * 100)</f>
-        <v>6.1403053815194388</v>
+        <f t="shared" si="0"/>
+        <v>6.5035713252942369</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -2606,14 +2675,14 @@
         <v>12</v>
       </c>
       <c r="B16">
-        <v>204647</v>
+        <v>220980</v>
       </c>
       <c r="D16" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="E16">
-        <f xml:space="preserve"> ((B17 - B16) / B16 * 100)</f>
-        <v>5.4185988555903579</v>
+        <f t="shared" si="0"/>
+        <v>6.1720517693908956</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2621,14 +2690,14 @@
         <v>13</v>
       </c>
       <c r="B17">
-        <v>215736</v>
+        <v>234619</v>
       </c>
       <c r="D17" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="E17">
-        <f xml:space="preserve"> ((B18 - B17) / B17 * 100)</f>
-        <v>5.414024548522268</v>
+        <f t="shared" si="0"/>
+        <v>5.6431917278651778</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2636,14 +2705,14 @@
         <v>11</v>
       </c>
       <c r="B18">
-        <v>227416</v>
+        <v>247859</v>
       </c>
       <c r="D18" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="E18">
-        <f xml:space="preserve"> ((B19 - B18) / B18 * 100)</f>
-        <v>4.8927955816653181</v>
+        <f t="shared" si="0"/>
+        <v>5.5329844790788316</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2651,14 +2720,14 @@
         <v>10</v>
       </c>
       <c r="B19">
-        <v>238543</v>
+        <v>261573</v>
       </c>
       <c r="D19" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="E19">
-        <f xml:space="preserve"> ((B20 - B19) / B19 * 100)</f>
-        <v>4.8138071542656879</v>
+        <f t="shared" si="0"/>
+        <v>5.1052669809192848</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -2666,10 +2735,7 @@
         <v>9</v>
       </c>
       <c r="B20">
-        <v>250026</v>
-      </c>
-      <c r="D20" t="s">
-        <v>9</v>
+        <v>274927</v>
       </c>
     </row>
   </sheetData>

</xml_diff>